<commit_message>
refactor trading analysis script to use yfinance for stock data retrieval and improve error handling
</commit_message>
<xml_diff>
--- a/ports/crypto_report.xlsx
+++ b/ports/crypto_report.xlsx
@@ -14,21 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>BTC-USD</t>
+  </si>
+  <si>
+    <t>Adj Close</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
   <si>
     <t>Open</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Adj Close</t>
   </si>
   <si>
     <t>Volume</t>
@@ -41,9 +50,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -96,12 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -157,85 +160,15 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>45474</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>45475</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>45476</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45477</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45478</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>45479</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45480</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45481</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45482</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45483</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>45484</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>Sheet1!$A$2:$A$1</c:f>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>62673.60546875</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62844.41015625</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>62034.33203125</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>60147.13671875</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>57022.80859375</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>56659.07421875</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>58239.4296875</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>55849.57421875</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>56704.59765625</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>58033.8828125</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>57729.890625</c:v>
-                </c:pt>
+                <c:ptCount val="0"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -642,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -652,282 +585,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="2">
-        <v>45474</v>
-      </c>
-      <c r="B2">
-        <v>62673.60546875</v>
-      </c>
-      <c r="C2">
-        <v>63777.2265625</v>
-      </c>
-      <c r="D2">
-        <v>62495.51171875</v>
-      </c>
-      <c r="E2">
-        <v>62851.98046875</v>
-      </c>
-      <c r="F2">
-        <v>62851.98046875</v>
-      </c>
-      <c r="G2">
-        <v>25468379421</v>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2">
-        <v>45475</v>
-      </c>
-      <c r="B3">
-        <v>62844.41015625</v>
-      </c>
-      <c r="C3">
-        <v>63203.359375</v>
-      </c>
-      <c r="D3">
-        <v>61752.74609375</v>
-      </c>
-      <c r="E3">
-        <v>62029.015625</v>
-      </c>
-      <c r="F3">
-        <v>62029.015625</v>
-      </c>
-      <c r="G3">
-        <v>20151616992</v>
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2">
-        <v>45476</v>
-      </c>
-      <c r="B4">
-        <v>62034.33203125</v>
-      </c>
-      <c r="C4">
-        <v>62187.703125</v>
-      </c>
-      <c r="D4">
-        <v>59419.38671875</v>
-      </c>
-      <c r="E4">
-        <v>60173.921875</v>
-      </c>
-      <c r="F4">
-        <v>60173.921875</v>
-      </c>
-      <c r="G4">
-        <v>29756701685</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="2">
-        <v>45477</v>
-      </c>
-      <c r="B5">
-        <v>60147.13671875</v>
-      </c>
-      <c r="C5">
-        <v>60399.67578125</v>
-      </c>
-      <c r="D5">
-        <v>56777.8046875</v>
-      </c>
-      <c r="E5">
-        <v>56977.703125</v>
-      </c>
-      <c r="F5">
-        <v>56977.703125</v>
-      </c>
-      <c r="G5">
-        <v>41149609230</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2">
-        <v>45478</v>
-      </c>
-      <c r="B6">
-        <v>57022.80859375</v>
-      </c>
-      <c r="C6">
-        <v>57497.15234375</v>
-      </c>
-      <c r="D6">
-        <v>53717.375</v>
-      </c>
-      <c r="E6">
-        <v>56662.375</v>
-      </c>
-      <c r="F6">
-        <v>56662.375</v>
-      </c>
-      <c r="G6">
-        <v>55417544033</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2">
-        <v>45479</v>
-      </c>
-      <c r="B7">
-        <v>56659.07421875</v>
-      </c>
-      <c r="C7">
-        <v>58472.546875</v>
-      </c>
-      <c r="D7">
-        <v>56038.9609375</v>
-      </c>
-      <c r="E7">
-        <v>58303.5390625</v>
-      </c>
-      <c r="F7">
-        <v>58303.5390625</v>
-      </c>
-      <c r="G7">
-        <v>20610320577</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="2">
-        <v>45480</v>
-      </c>
-      <c r="B8">
-        <v>58239.4296875</v>
-      </c>
-      <c r="C8">
-        <v>58371.12109375</v>
-      </c>
-      <c r="D8">
-        <v>55793.32421875</v>
-      </c>
-      <c r="E8">
-        <v>55849.109375</v>
-      </c>
-      <c r="F8">
-        <v>55849.109375</v>
-      </c>
-      <c r="G8">
-        <v>20553359505</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2">
-        <v>45481</v>
-      </c>
-      <c r="B9">
-        <v>55849.57421875</v>
-      </c>
-      <c r="C9">
-        <v>58131.3359375</v>
-      </c>
-      <c r="D9">
-        <v>54321.01953125</v>
-      </c>
-      <c r="E9">
-        <v>56705.09765625</v>
-      </c>
-      <c r="F9">
-        <v>56705.09765625</v>
-      </c>
-      <c r="G9">
-        <v>39766159899</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="2">
-        <v>45482</v>
-      </c>
-      <c r="B10">
-        <v>56704.59765625</v>
-      </c>
-      <c r="C10">
-        <v>58239.1953125</v>
-      </c>
-      <c r="D10">
-        <v>56316.875</v>
-      </c>
-      <c r="E10">
-        <v>58009.2265625</v>
-      </c>
-      <c r="F10">
-        <v>58009.2265625</v>
-      </c>
-      <c r="G10">
-        <v>27849512607</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="2">
-        <v>45483</v>
-      </c>
-      <c r="B11">
-        <v>58033.8828125</v>
-      </c>
-      <c r="C11">
-        <v>59359.43359375</v>
-      </c>
-      <c r="D11">
-        <v>57178.4140625</v>
-      </c>
-      <c r="E11">
-        <v>57742.49609375</v>
-      </c>
-      <c r="F11">
-        <v>57742.49609375</v>
-      </c>
-      <c r="G11">
-        <v>26175260526</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2">
-        <v>45484</v>
-      </c>
-      <c r="B12">
-        <v>57729.890625</v>
-      </c>
-      <c r="C12">
-        <v>59299.43359375</v>
-      </c>
-      <c r="D12">
-        <v>57120.37890625</v>
-      </c>
-      <c r="E12">
-        <v>57344.9140625</v>
-      </c>
-      <c r="F12">
-        <v>57344.9140625</v>
-      </c>
-      <c r="G12">
-        <v>28707803842</v>
+      <c r="A4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>